<commit_message>
Added results and Figures
</commit_message>
<xml_diff>
--- a/DataSets/BotResultsSimple.xlsx
+++ b/DataSets/BotResultsSimple.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\Dissertation_Artefact\DataSets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC88CA10-CB63-46AA-9361-86743AE8F07F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E5EEF0-32E8-4F46-B5D4-6258639F62EE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12210" xr2:uid="{F1EB8304-46E2-4A3C-AA5D-ED017799EB4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Bot</t>
   </si>
@@ -79,13 +79,16 @@
   </si>
   <si>
     <t>Oritaka</t>
+  </si>
+  <si>
+    <t>POSH-core</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +106,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
@@ -198,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -230,6 +239,16 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -550,15 +569,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811D39B2-9CC8-4759-A1B7-EFB6A8FA04B7}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K10"/>
+      <selection activeCell="K2" sqref="K2:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -586,25 +605,29 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>9</v>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+    </row>
+    <row r="2" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="B2" s="5">
         <v>80</v>
       </c>
       <c r="C2" s="5">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D2" s="5">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E2" s="5">
-        <v>85</v>
-      </c>
-      <c r="F2" s="11">
-        <v>13.03</v>
+        <v>91.25</v>
+      </c>
+      <c r="F2" s="15">
+        <v>6.25</v>
       </c>
       <c r="G2" s="5">
         <v>0</v>
@@ -615,29 +638,32 @@
       <c r="I2" s="5">
         <v>0</v>
       </c>
+      <c r="J2" s="14"/>
       <c r="K2" s="6"/>
-    </row>
-    <row r="3" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8">
+        <v>79</v>
+      </c>
+      <c r="C3" s="8">
+        <v>69</v>
+      </c>
+      <c r="D3" s="8">
         <v>10</v>
       </c>
-      <c r="B3" s="8">
-        <v>80</v>
-      </c>
-      <c r="C3" s="8">
-        <v>68</v>
-      </c>
-      <c r="D3" s="8">
-        <v>12</v>
-      </c>
       <c r="E3" s="8">
-        <v>85</v>
-      </c>
-      <c r="F3" s="12">
-        <v>6.05</v>
+        <v>87.34</v>
+      </c>
+      <c r="F3" s="16">
+        <v>13.13</v>
       </c>
       <c r="G3" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="8">
         <v>0</v>
@@ -645,29 +671,32 @@
       <c r="I3" s="8">
         <v>0</v>
       </c>
+      <c r="J3" s="14"/>
       <c r="K3" s="9"/>
-    </row>
-    <row r="4" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+    </row>
+    <row r="4" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="5">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C4" s="5">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D4" s="5">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E4" s="5">
-        <v>68.75</v>
-      </c>
-      <c r="F4" s="11">
-        <v>14.09</v>
+        <v>74.069999999999993</v>
+      </c>
+      <c r="F4" s="15">
+        <v>11.58</v>
       </c>
       <c r="G4" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H4" s="5">
         <v>0</v>
@@ -675,9 +704,12 @@
       <c r="I4" s="5">
         <v>0</v>
       </c>
+      <c r="J4" s="14"/>
       <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+    </row>
+    <row r="5" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>12</v>
       </c>
@@ -685,106 +717,115 @@
         <v>80</v>
       </c>
       <c r="C5" s="8">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D5" s="8">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E5" s="8">
-        <v>56.25</v>
-      </c>
-      <c r="F5" s="12">
-        <v>15.53</v>
+        <v>60</v>
+      </c>
+      <c r="F5" s="16">
+        <v>16.11</v>
       </c>
       <c r="G5" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H5" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I5" s="8">
         <v>0</v>
       </c>
+      <c r="J5" s="14"/>
       <c r="K5" s="9"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>13</v>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+    </row>
+    <row r="6" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="B6" s="5">
         <v>80</v>
       </c>
       <c r="C6" s="5">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D6" s="5">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E6" s="5">
-        <v>53.75</v>
-      </c>
-      <c r="F6" s="11">
-        <v>14.33</v>
+        <v>56.25</v>
+      </c>
+      <c r="F6" s="15">
+        <v>14.31</v>
       </c>
       <c r="G6" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H6" s="5">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I6" s="5">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J6" s="14"/>
       <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>14</v>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B7" s="8">
         <v>80</v>
       </c>
       <c r="C7" s="8">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="8">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E7" s="8">
-        <v>47.5</v>
-      </c>
-      <c r="F7" s="12">
-        <v>13.28</v>
+        <v>46.25</v>
+      </c>
+      <c r="F7" s="16">
+        <v>14.31</v>
       </c>
       <c r="G7" s="8">
         <v>2</v>
       </c>
       <c r="H7" s="8">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I7" s="8">
-        <v>7</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J7" s="14"/>
       <c r="K7" s="9"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="5">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" s="5">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D8" s="5">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E8" s="5">
-        <v>25</v>
-      </c>
-      <c r="F8" s="11">
-        <v>17.100000000000001</v>
+        <v>34.18</v>
+      </c>
+      <c r="F8" s="15">
+        <v>15.56</v>
       </c>
       <c r="G8" s="5">
         <v>5</v>
@@ -795,9 +836,12 @@
       <c r="I8" s="5">
         <v>0</v>
       </c>
+      <c r="J8" s="14"/>
       <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+    </row>
+    <row r="9" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>16</v>
       </c>
@@ -805,57 +849,117 @@
         <v>80</v>
       </c>
       <c r="C9" s="8">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D9" s="8">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E9" s="8">
-        <v>17.5</v>
-      </c>
-      <c r="F9" s="12">
-        <v>19.239999999999998</v>
+        <v>22.5</v>
+      </c>
+      <c r="F9" s="16">
+        <v>18.02</v>
       </c>
       <c r="G9" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H9" s="8">
         <v>0</v>
       </c>
       <c r="I9" s="8">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J9" s="14"/>
       <c r="K9" s="9"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="5">
+        <v>81</v>
+      </c>
+      <c r="C10" s="5">
+        <v>15</v>
+      </c>
+      <c r="D10" s="5">
+        <v>66</v>
+      </c>
+      <c r="E10" s="5">
+        <v>18.52</v>
+      </c>
+      <c r="F10" s="15">
+        <v>17.22</v>
+      </c>
+      <c r="G10" s="5">
+        <v>9</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="14"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+    </row>
+    <row r="11" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="8">
         <v>80</v>
       </c>
-      <c r="C10" s="5">
-        <v>9</v>
-      </c>
-      <c r="D10" s="5">
-        <v>71</v>
-      </c>
-      <c r="E10" s="5">
-        <v>11.25</v>
-      </c>
-      <c r="F10" s="11">
-        <v>15.2</v>
-      </c>
-      <c r="G10" s="5">
-        <v>4</v>
-      </c>
-      <c r="H10" s="5">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5">
-        <v>0</v>
-      </c>
-      <c r="K10" s="6"/>
+      <c r="C11" s="8">
+        <v>8</v>
+      </c>
+      <c r="D11" s="8">
+        <v>72</v>
+      </c>
+      <c r="E11" s="8">
+        <v>10</v>
+      </c>
+      <c r="F11" s="16">
+        <v>16.239999999999998</v>
+      </c>
+      <c r="G11" s="8">
+        <v>7</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0</v>
+      </c>
+      <c r="J11" s="14"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>